<commit_message>
optimization algorithm is updated (price and index problem)
</commit_message>
<xml_diff>
--- a/WH_Amounts.xlsx
+++ b/WH_Amounts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <x:si>
     <x:t>Materials</x:t>
   </x:si>
@@ -28,9 +28,6 @@
     <x:t>WareHouse 2</x:t>
   </x:si>
   <x:si>
-    <x:t>WareHouse 3</x:t>
-  </x:si>
-  <x:si>
     <x:t>TotalCost</x:t>
   </x:si>
   <x:si>
@@ -40,51 +37,51 @@
     <x:t>WareHouse 6</x:t>
   </x:si>
   <x:si>
+    <x:t>100</x:t>
+  </x:si>
+  <x:si>
     <x:t>125</x:t>
   </x:si>
   <x:si>
+    <x:t>350</x:t>
+  </x:si>
+  <x:si>
+    <x:t>550</x:t>
+  </x:si>
+  <x:si>
+    <x:t>175</x:t>
+  </x:si>
+  <x:si>
     <x:t>200</x:t>
   </x:si>
   <x:si>
-    <x:t>225</x:t>
-  </x:si>
-  <x:si>
-    <x:t>550</x:t>
-  </x:si>
-  <x:si>
-    <x:t>175</x:t>
-  </x:si>
-  <x:si>
     <x:t>975</x:t>
   </x:si>
   <x:si>
+    <x:t>AEB1</x:t>
+  </x:si>
+  <x:si>
     <x:t>AEC1</x:t>
   </x:si>
   <x:si>
+    <x:t>AEC3</x:t>
+  </x:si>
+  <x:si>
     <x:t>AEC4</x:t>
   </x:si>
   <x:si>
-    <x:t>AED1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AEC3</x:t>
-  </x:si>
-  <x:si>
     <x:t>MN17-G2</x:t>
   </x:si>
   <x:si>
-    <x:t>21336</x:t>
+    <x:t>21335</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
   </x:si>
   <x:si>
     <x:t>21000</x:t>
   </x:si>
   <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
     <x:t>110</x:t>
   </x:si>
   <x:si>
@@ -94,7 +91,10 @@
     <x:t>520</x:t>
   </x:si>
   <x:si>
-    <x:t>100</x:t>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>516</x:t>
   </x:si>
   <x:si>
     <x:t>BL2137</x:t>
@@ -104,9 +104,6 @@
   </x:si>
   <x:si>
     <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>360</x:t>
   </x:si>
   <x:si>
     <x:t>51</x:t>
@@ -597,36 +594,36 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
+      <x:c r="H1" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="I1" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:9">
       <x:c r="C2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>12</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>9</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
         <x:v>13</x:v>
@@ -639,14 +636,11 @@
       <x:c r="D3" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
+      <x:c r="G3" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
+      <x:c r="H3" s="0" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
@@ -662,37 +656,31 @@
       <x:c r="D4" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
+      <x:c r="G4" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:9">
       <x:c r="A5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>25</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:9">
@@ -703,444 +691,441 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:9">
       <x:c r="G7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:9"/>
     <x:row r="9" spans="1:9">
       <x:c r="A9" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
       <x:c r="A10" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:9">
       <x:c r="A11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
+      <x:c r="C11" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C11" s="0" t="s">
+      <x:c r="D11" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="E11" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="E11" s="0" t="s">
+      <x:c r="F11" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="F11" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
       <x:c r="A12" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:9">
       <x:c r="A13" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:9">
       <x:c r="A14" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:9">
       <x:c r="A15" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:9">
       <x:c r="A16" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:9">
       <x:c r="A17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="B17" s="0" t="s">
+      <x:c r="C17" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="C17" s="0" t="s">
+      <x:c r="D17" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:9">
       <x:c r="A18" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="B18" s="0" t="s">
+      <x:c r="C18" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:9">
       <x:c r="A19" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:9">
       <x:c r="A20" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="B20" s="0" t="s">
+      <x:c r="C20" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:9">
       <x:c r="A21" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:9">
       <x:c r="A22" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="H22" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:9">
       <x:c r="A23" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H23" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:9">
       <x:c r="A24" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="H24" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:9"/>

</xml_diff>